<commit_message>
Small changes in project and big changes in document.
</commit_message>
<xml_diff>
--- a/DefenceOfTheAncientsRPG/DefenceOfTheAncientsRPG/wwwroot/addContentTemplates/item-template.xlsx
+++ b/DefenceOfTheAncientsRPG/DefenceOfTheAncientsRPG/wwwroot/addContentTemplates/item-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruudd\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruudd\source\repos\dota2rpg\DefenceOfTheAncientsRPG\DefenceOfTheAncientsRPG\wwwroot\addContentTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D870D725-B028-413C-A504-FA6D4808AD78}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AAA20F-3828-4E70-8335-588AE26765A8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7725" windowHeight="7980" xr2:uid="{1D94DD81-E627-4215-84AA-0CDE563F018D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t xml:space="preserve"> | Add new content here</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> | </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> v</t>
   </si>
 </sst>
 </file>
@@ -463,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D346AF-AAE5-428F-835C-886AB7847D3E}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,16 +520,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>